<commit_message>
Organize codebase structure for production deployment
- Move non-production files to archived folders
- Clean up data directory structure
- Update .gitignore for better file management
- Organize scripts and SQL files into appropriate folders
- Maintain clear separation between production and development files

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/raw/coversion factors.xlsx
+++ b/data/raw/coversion factors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\Data_Science_Projects\petroverse\petroverse_analytics\cleaned_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\Data_Science_Projects\petroverse_analytics\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF3B822-7E4B-4465-AD63-D82AE1BEFD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B0D21-1854-4960-82AD-FB05E8C3FDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1828FAD-DCFD-43DD-BCCD-F16E00540743}"/>
   </bookViews>
@@ -36,37 +36,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Fuel  oil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas oil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marine Gasoil </t>
-  </si>
-  <si>
-    <t>Unified</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Kerosene </t>
   </si>
   <si>
+    <t xml:space="preserve">Premix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATK </t>
+  </si>
+  <si>
+    <t>Conversion Factor (CF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gasoline </t>
+  </si>
+  <si>
+    <t>Gasoil</t>
+  </si>
+  <si>
     <t xml:space="preserve">LPG </t>
   </si>
   <si>
-    <t xml:space="preserve">Premium </t>
-  </si>
-  <si>
-    <t>Conversion Factor</t>
+    <t>LPG CRM</t>
+  </si>
+  <si>
+    <t>Marine Gasoil Local</t>
+  </si>
+  <si>
+    <t>Marine Gasoil Foreign</t>
+  </si>
+  <si>
+    <t>Gasoil Mines</t>
+  </si>
+  <si>
+    <t>Gasoil Rig</t>
+  </si>
+  <si>
+    <t>Gasoil Power Plant</t>
+  </si>
+  <si>
+    <t>Gasoil Cell Site</t>
+  </si>
+  <si>
+    <t>Fuel Oil Industrial</t>
+  </si>
+  <si>
+    <t>Fuel Oil Power Plant</t>
+  </si>
+  <si>
+    <t>Naphtha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,29 +102,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -105,14 +154,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,74 +573,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5898C5BA-E92B-4841-9501-CB777444284E}">
-  <dimension ref="B1:I2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1005.03</v>
-      </c>
-      <c r="D2" s="2">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9">
+        <v>1324.5</v>
+      </c>
+      <c r="D2" s="10">
         <v>1183.43</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="10">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1324.5</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1240.5999999999999</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1240.5999999999999</v>
+      </c>
+      <c r="J2" s="10">
         <v>1183.43</v>
       </c>
-      <c r="F2" s="2">
-        <v>1342.28</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1240.5999999999999</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1342.28</v>
-      </c>
+      <c r="K2" s="10">
+        <v>1183.43</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1183.43</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1183.43</v>
+      </c>
+      <c r="N2" s="10">
+        <v>1183.43</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1183.43</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1009.08</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>1009.08</v>
+      </c>
+      <c r="R2" s="10">
+        <v>1324.5</v>
+      </c>
+      <c r="S2" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>